<commit_message>
update latest version to 1.7.0
</commit_message>
<xml_diff>
--- a/run/input.xlsx
+++ b/run/input.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,6 +483,18 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>smtp_from_user_nickname</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>AIjiaRobot</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
update latest version to 1.8.1
</commit_message>
<xml_diff>
--- a/run/input.xlsx
+++ b/run/input.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -54,18 +54,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -398,7 +398,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>yanan.chen@net263.com,lipeng.sun@net263.com,shilong.zhai@net263.com,hao1.li@net263.com, yueheng.wu@net263.com, huanghe.luo@net263.com, zilin.niu@net263.com,KeithXi &lt;xiaofeng.xi@net263.com&gt;,fsha@net263.com,cshen@net263.com,nan.zhang@net263.com,chengkun.liu@net263.com,tiezhou.wei@net263.com,haichao.lu@net263.com,yuanlong.li@net263.com</t>
+          <t>&lt;吴岳恒&gt;yueheng.wu@net263.com,&lt;李浩&gt;hao1.li@net263.com,&lt;KeithXi&gt;xiaofeng.xi@net263.com</t>
         </is>
       </c>
     </row>
@@ -496,6 +496,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>